<commit_message>
Rename and add features
</commit_message>
<xml_diff>
--- a/excel_input/KEY ORGANIZERS.xlsx
+++ b/excel_input/KEY ORGANIZERS.xlsx
@@ -5,15 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared Documents/IT Development/Contacts Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pytest\excel_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_13AD86F674413BE0E470FD5D1A1C692472DEC0CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBD6BAD4-1630-40C6-8A4B-907BE16DBE4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FEB88F-ABDE-42B7-B00D-405595AC70E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="17376" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="IT TEAM" sheetId="1" r:id="rId1"/>
+    <sheet name="LEADERS" sheetId="2" r:id="rId1"/>
+    <sheet name="OPERATIONS TEAM" sheetId="3" r:id="rId2"/>
+    <sheet name="FINANCE TEAM" sheetId="4" r:id="rId3"/>
+    <sheet name="PARTNER EXPERIENCE TEAM" sheetId="5" r:id="rId4"/>
+    <sheet name="STUDENT SUCCESS TEAM" sheetId="6" r:id="rId5"/>
+    <sheet name="IT DEVELOPMENT TEAM" sheetId="1" r:id="rId6"/>
+    <sheet name="MARKETING &amp; COMMUNICATIONS TEAM" sheetId="7" r:id="rId7"/>
+    <sheet name="CREATIVES TEAM" sheetId="8" r:id="rId8"/>
+    <sheet name="CONSULTANTS" sheetId="9" r:id="rId9"/>
+    <sheet name="ISSUE MANAGEMENT TEAM" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="348">
   <si>
     <t>Name</t>
   </si>
@@ -211,84 +220,886 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>=VLOOKUP(B2,'[Hackathon 2025 Organizing Team Member Profile Submission.xlsx]Sheet1'!OfficeForms.Table[[Email]:[LinkedIn Profile]],4,FALSE</t>
-  </si>
-  <si>
     <t>Business Analyst</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/small_Guilherme%20Luiz%20Barbo.jpeg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/DSC_0011_Khassan%20Suleimanov.jpg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/IMG_2429_Mustafa%20Siddiqui.jpeg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/d1588d2d-1903-4b01-a6e3-f01a00a6d14f_Sam%20Alavi.jpeg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/Linkedin_Chonticha%20Praditsaku.jpg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/image_Shanu%20Anie%20Alias.png</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/IMG_4856_Ankit%20Thapar.jpeg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/DSC01890_Osman%20Kahraman.jpg</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/MPP_Abdulgafar%20Temitope.png</t>
+  </si>
+  <si>
+    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/000125130002_Boyu%20Cao.jpg</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rahul-mamania/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/guilhermebdasilva/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/khassan-suleimanov-494591254?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/mu5h1e</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/alavi-sam</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chonticha-praditsakul-67a629132/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shanu-anie-alias</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ankit-thapar-417873275</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/osman-kahraman-2a6513220</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/clevertag/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/xeoncao/</t>
+  </si>
+  <si>
     <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/WhatsApp%20Image%202024-10-30%20at%2023.19.35_Rahul%20Amish%20Mamania.jpeg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/small_Guilherme%20Luiz%20Barbo.jpeg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/DSC_0011_Khassan%20Suleimanov.jpg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/IMG_2429_Mustafa%20Siddiqui.jpeg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/d1588d2d-1903-4b01-a6e3-f01a00a6d14f_Sam%20Alavi.jpeg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/Linkedin_Chonticha%20Praditsaku.jpg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/image_Shanu%20Anie%20Alias.png</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/IMG_4856_Ankit%20Thapar.jpeg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/DSC01890_Osman%20Kahraman.jpg</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/MPP_Abdulgafar%20Temitope.png</t>
-  </si>
-  <si>
-    <t>https://seneca.sharepoint.com/sites/2025HackathonPlanning/Shared%20Documents/Apps/Microsoft%20Forms/Hackathon%202025%20Organizing%20Team%20Member%20Profile%20Subm/Question/000125130002_Boyu%20Cao.jpg</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/rahul-mamania/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/guilhermebdasilva/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/khassan-suleimanov-494591254?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/mu5h1e</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/alavi-sam</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/chonticha-praditsakul-67a629132/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/shanu-anie-alias</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ankit-thapar-417873275</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/osman-kahraman-2a6513220</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/clevertag/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/xeoncao/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mark Buchner</t>
+  </si>
+  <si>
+    <t>mark.buchner@senecapolytechnic.ca</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Suhana Shrestha</t>
+  </si>
+  <si>
+    <t>sshrestha140@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Chief of Staff</t>
+  </si>
+  <si>
+    <t>Irus Majam</t>
+  </si>
+  <si>
+    <t>icmajam@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Event Director</t>
+  </si>
+  <si>
+    <t>Umar Nazarin Packeer</t>
+  </si>
+  <si>
+    <t>unpackeer@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Project Manager, Operations</t>
+  </si>
+  <si>
+    <t>Ashmy Thomas</t>
+  </si>
+  <si>
+    <t>athomas141@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Daily Reports Officer</t>
+  </si>
+  <si>
+    <t>Weekly Operations Updates /Registration Team</t>
+  </si>
+  <si>
+    <t>Shikha Thing</t>
+  </si>
+  <si>
+    <t>sthing2@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Weekly Reports Officer</t>
+  </si>
+  <si>
+    <t>Integration Management / Project Control Officer</t>
+  </si>
+  <si>
+    <t>Jasmeen Kaur</t>
+  </si>
+  <si>
+    <t>jasmeen-kaur39@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Rules, Regulations, Prizing, and Judging </t>
+  </si>
+  <si>
+    <t>Stage Management</t>
+  </si>
+  <si>
+    <t>Nischal Sapkota</t>
+  </si>
+  <si>
+    <t>nsapkota5@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Prizing</t>
+  </si>
+  <si>
+    <t>Keerthivaasan Elango</t>
+  </si>
+  <si>
+    <t>kelango1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Judging</t>
+  </si>
+  <si>
+    <t>Procurement Team</t>
+  </si>
+  <si>
+    <t>Divanshu</t>
+  </si>
+  <si>
+    <t>divanshu2@myseneca.ca</t>
+  </si>
+  <si>
+    <t>School Facilities Liaison</t>
+  </si>
+  <si>
+    <t>Winlyn Luena</t>
+  </si>
+  <si>
+    <t>wluena@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Event SWAG</t>
+  </si>
+  <si>
+    <t>Procurement Team (Food / Merchandise)</t>
+  </si>
+  <si>
+    <t>Sanam Maharjan</t>
+  </si>
+  <si>
+    <t>smaharjan23@myseneca.ca</t>
+  </si>
+  <si>
+    <t>SWAG Officer</t>
+  </si>
+  <si>
+    <t>Procurement Team (SWAG / Supplies)</t>
+  </si>
+  <si>
+    <t>Nisal Chandana Ekanayake</t>
+  </si>
+  <si>
+    <t>ncekanayake@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Event Catering</t>
+  </si>
+  <si>
+    <t>Upesha Pankajbhai Patel</t>
+  </si>
+  <si>
+    <t>uppatel8@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Catering Officer</t>
+  </si>
+  <si>
+    <t>Naitik Pankaj Kumar Raval</t>
+  </si>
+  <si>
+    <t>npkraval@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Registrations</t>
+  </si>
+  <si>
+    <t>Registration Team</t>
+  </si>
+  <si>
+    <t>Harmanjot Singh</t>
+  </si>
+  <si>
+    <t>hsingh958@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Registration Officer</t>
+  </si>
+  <si>
+    <t>Andrea Huesca Enciso</t>
+  </si>
+  <si>
+    <t>ahuesca-enciso@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Broadcast Officer</t>
+  </si>
+  <si>
+    <t>Event and Media Production</t>
+  </si>
+  <si>
+    <t>Broadcast Team</t>
+  </si>
+  <si>
+    <t>Brenda Cáceres</t>
+  </si>
+  <si>
+    <t>cvbrenda@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Haru Ai Okabe</t>
+  </si>
+  <si>
+    <t>haokabe@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Khushi Ajit Vaswani</t>
+  </si>
+  <si>
+    <t>kvaswani1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Microcredentials</t>
+  </si>
+  <si>
+    <t>Business Tech Management</t>
+  </si>
+  <si>
+    <t>Ramesh Banjade</t>
+  </si>
+  <si>
+    <t>rbanjade@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Operations Officer</t>
+  </si>
+  <si>
+    <t>Runner</t>
+  </si>
+  <si>
+    <t>Biplav Neupane</t>
+  </si>
+  <si>
+    <t>bneupane9@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Sagar Yonjan</t>
+  </si>
+  <si>
+    <t>slama12@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Seyedesomaye Najafi (Samira)</t>
+  </si>
+  <si>
+    <t>snajafi6@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Manager, Event Accounting </t>
+  </si>
+  <si>
+    <t>Finance Planning</t>
+  </si>
+  <si>
+    <t>Fenil Mehta</t>
+  </si>
+  <si>
+    <t>fmmehta@myseneca.ca</t>
+  </si>
+  <si>
+    <t>P.E / Operations</t>
+  </si>
+  <si>
+    <t>Director, Partner Experience</t>
+  </si>
+  <si>
+    <t>Lily Ngo</t>
+  </si>
+  <si>
+    <t>lhngo1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Partner Experience</t>
+  </si>
+  <si>
+    <t>Manager, Corporate Relations</t>
+  </si>
+  <si>
+    <t>Corporate Relations</t>
+  </si>
+  <si>
+    <t>Abhinaya Narayanan Subramanian</t>
+  </si>
+  <si>
+    <t>anarayanan-subramani@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Project Control Officer. Partner Exp.</t>
+  </si>
+  <si>
+    <t>Abigail Cabazal</t>
+  </si>
+  <si>
+    <t>acabazal@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Partner Exp. Officer</t>
+  </si>
+  <si>
+    <t>Justin Chu</t>
+  </si>
+  <si>
+    <t>hychu2@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Not-For-Profit Relations</t>
+  </si>
+  <si>
+    <t>Business Management</t>
+  </si>
+  <si>
+    <t>Non-Profit Organizations</t>
+  </si>
+  <si>
+    <t>Shreet Ketan Dave</t>
+  </si>
+  <si>
+    <t>skdave@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Krishita Nirmesh Vakil</t>
+  </si>
+  <si>
+    <t>knvakil@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, WIL Coordination</t>
+  </si>
+  <si>
+    <t>Seneca Works</t>
+  </si>
+  <si>
+    <t>Manjot Singh</t>
+  </si>
+  <si>
+    <t>msingh802@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Abhishek Pal</t>
+  </si>
+  <si>
+    <t>apal21@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Mankomal Kaur Gandhara</t>
+  </si>
+  <si>
+    <t>mkgandhara@myseneca.ca</t>
+  </si>
+  <si>
+    <t>BSA</t>
+  </si>
+  <si>
+    <t>Jay Vijaykumar Vakil</t>
+  </si>
+  <si>
+    <t>jvakil@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Government Relations</t>
+  </si>
+  <si>
+    <t>Government Relations</t>
+  </si>
+  <si>
+    <t>Subhankar Gon</t>
+  </si>
+  <si>
+    <t>sgon@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Ayush Shah</t>
+  </si>
+  <si>
+    <t>ayushshahas17@outlook.com</t>
+  </si>
+  <si>
+    <t>Information Technology Solutions</t>
+  </si>
+  <si>
+    <t>Kris Sadiasa</t>
+  </si>
+  <si>
+    <t>kalmodal@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Student Success</t>
+  </si>
+  <si>
+    <t>Student Success Director</t>
+  </si>
+  <si>
+    <t>Computer System Technology</t>
+  </si>
+  <si>
+    <t>Rui Zhu (Hathaway)</t>
+  </si>
+  <si>
+    <t>rzhu27@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Challenge Set Liaison / Team Lead – Participant Support</t>
+  </si>
+  <si>
+    <t>Bachelor of Data Science and Analytics</t>
+  </si>
+  <si>
+    <t>Ameya Mangesh Kokatay</t>
+  </si>
+  <si>
+    <t>ameya-mangesh.kokatay@senecapolytechnic.ca</t>
+  </si>
+  <si>
+    <t>Student Sucess Manager</t>
+  </si>
+  <si>
+    <t>Tomisin Jephthah Ojaokomo</t>
+  </si>
+  <si>
+    <t>tjojaokomo@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Discord &amp; Ticketing System Manager</t>
+  </si>
+  <si>
+    <t>Syed Shahzeb Saleem</t>
+  </si>
+  <si>
+    <t>sssaleem@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Conflict Resolution Manager</t>
+  </si>
+  <si>
+    <t>Susma Thapa</t>
+  </si>
+  <si>
+    <t>sthapa57@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Conflict Resolution Officer</t>
+  </si>
+  <si>
+    <t>Early Childhood Education</t>
+  </si>
+  <si>
+    <t>W Dinithi Indrachaya Fernando</t>
+  </si>
+  <si>
+    <t>wdifernando@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Student Sucess Officer</t>
+  </si>
+  <si>
+    <t>Rashidat Kolawole</t>
+  </si>
+  <si>
+    <t>rskolawole@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Colleges, Universities and Seneca</t>
+  </si>
+  <si>
+    <t>Devanshi Bharatkumar Lokhandwala</t>
+  </si>
+  <si>
+    <t>dblokhandwala@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Jenil Hirenkumar Mehta</t>
+  </si>
+  <si>
+    <t>jhmehta1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Nicole Herman Rodrigues</t>
+  </si>
+  <si>
+    <t>nhrodrigues@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Mai Huong Nguyen</t>
+  </si>
+  <si>
+    <t>mhnguyen23@myseneca.ca</t>
+  </si>
+  <si>
+    <t>SCM</t>
+  </si>
+  <si>
+    <t>Sarthak Gupta</t>
+  </si>
+  <si>
+    <t>sgupta1797@conestogac.on.ca</t>
+  </si>
+  <si>
+    <t>Web development</t>
+  </si>
+  <si>
+    <t>Shakila Samaradiwakara</t>
+  </si>
+  <si>
+    <t>Ssamaradiwakara6070@conestogac.on.ca</t>
+  </si>
+  <si>
+    <t>Utpal Manishchandra Prajapati</t>
+  </si>
+  <si>
+    <t>umprajapati@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Dwayne Jude Saldanha</t>
+  </si>
+  <si>
+    <t>djsaldanha@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Vladyslav Savchyn</t>
+  </si>
+  <si>
+    <t>vsavchyn@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Arafat Ahmed Ansari</t>
+  </si>
+  <si>
+    <t>aa8@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Project Manager, Marketing</t>
+  </si>
+  <si>
+    <t>Podcast Manager</t>
+  </si>
+  <si>
+    <t>Umut Deniz Eryigit</t>
+  </si>
+  <si>
+    <t>uderyigit@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Motion Graphics</t>
+  </si>
+  <si>
+    <t>Graphics Design</t>
+  </si>
+  <si>
+    <t>Master of Ceremony (Mixers, Quali, Finale)</t>
+  </si>
+  <si>
+    <t>Dinh Quoc</t>
+  </si>
+  <si>
+    <t>dto8@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Graphics Designer</t>
+  </si>
+  <si>
+    <t>Social Media Manager</t>
+  </si>
+  <si>
+    <t>Chan Young Kim</t>
+  </si>
+  <si>
+    <t>cykim4@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Website Manager (Website Content)</t>
+  </si>
+  <si>
+    <t>Talia Ghalayini</t>
+  </si>
+  <si>
+    <t>tghalayini1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Manager, Communication</t>
+  </si>
+  <si>
+    <t>Computer Engineering Technology</t>
+  </si>
+  <si>
+    <t>Communication manager</t>
+  </si>
+  <si>
+    <t>Justice Asiedu</t>
+  </si>
+  <si>
+    <t>jasiedu1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Communications Officer</t>
+  </si>
+  <si>
+    <t>Vidhi Mehta</t>
+  </si>
+  <si>
+    <t>vidhi236@my.yorku.ca</t>
+  </si>
+  <si>
+    <t>Manager, Marketing Strategy</t>
+  </si>
+  <si>
+    <t>Digital Marketing</t>
+  </si>
+  <si>
+    <t>Print Manager*</t>
+  </si>
+  <si>
+    <t>Zoe Lara Denise Lerin</t>
+  </si>
+  <si>
+    <t>zldlerin@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Queen of Hackathon</t>
+  </si>
+  <si>
+    <t>Mohammad Mozaffari</t>
+  </si>
+  <si>
+    <t>mmozaffri@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Content Creators</t>
+  </si>
+  <si>
+    <t>Internation Business</t>
+  </si>
+  <si>
+    <t>Content Creator</t>
+  </si>
+  <si>
+    <t>Ayda Safiri</t>
+  </si>
+  <si>
+    <t>asafiri1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Mobina Kazemi</t>
+  </si>
+  <si>
+    <t>kmobina@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Aayushi Mahendra Sharma</t>
+  </si>
+  <si>
+    <t>amsharma1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Content Lead</t>
+  </si>
+  <si>
+    <t>Justin Wong</t>
+  </si>
+  <si>
+    <t>jwong301@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Copywriter</t>
+  </si>
+  <si>
+    <t>Public Relations and Communications</t>
+  </si>
+  <si>
+    <t>Pavan Kumar</t>
+  </si>
+  <si>
+    <t>pavan108@my.yorku.ca</t>
+  </si>
+  <si>
+    <t>Manager, Content Strategy</t>
+  </si>
+  <si>
+    <t>Safal Maharjan</t>
+  </si>
+  <si>
+    <t>smaharjan34@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Video Editor</t>
+  </si>
+  <si>
+    <t>Branding Manager (Should be with creatives)</t>
+  </si>
+  <si>
+    <t>Winona Putri Wirindra</t>
+  </si>
+  <si>
+    <t>wpwirindra@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Videographer/Video editor</t>
+  </si>
+  <si>
+    <t>Creative Advertising</t>
+  </si>
+  <si>
+    <t>Vanshil Lukhad</t>
+  </si>
+  <si>
+    <t>vlukhad@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Visual Content Creation</t>
+  </si>
+  <si>
+    <t>Kaifee Ali</t>
+  </si>
+  <si>
+    <t>kali64@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Le Xuan Hoa Dao (Hannah)</t>
+  </si>
+  <si>
+    <t>lxhdao@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Designing</t>
+  </si>
+  <si>
+    <t>Creative Director</t>
+  </si>
+  <si>
+    <t>Graphic Design</t>
+  </si>
+  <si>
+    <t>Edwin Ramirez</t>
+  </si>
+  <si>
+    <t>eramierez@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Merchandise Lead Designer</t>
+  </si>
+  <si>
+    <t>Sanabanu Basir Patel (Sana)</t>
+  </si>
+  <si>
+    <t>sbpatel52@myseneca.ca</t>
+  </si>
+  <si>
+    <t>UI/UX Lead Designer</t>
+  </si>
+  <si>
+    <t>Marketing / Partner Experience</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Social Media Marketing</t>
+  </si>
+  <si>
+    <t>IT / Student Success/ First Nations</t>
+  </si>
+  <si>
+    <t>BSD</t>
+  </si>
+  <si>
+    <t>Rishan Mendis</t>
+  </si>
+  <si>
+    <t>rishanmendis@yahoo.com / rmendis1@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Shreya Adhvaryu</t>
+  </si>
+  <si>
+    <t>shreya.adhvaryu@senecapolytechnic.ca</t>
+  </si>
+  <si>
+    <t>Shlok Kumar Sharma</t>
+  </si>
+  <si>
+    <t>shlok-kumar.sharma@senecapolytechnic.ca</t>
+  </si>
+  <si>
+    <t>Arya Prasad Samant</t>
+  </si>
+  <si>
+    <t>aryasamant.10@gmail.com</t>
+  </si>
+  <si>
+    <t>Majd Al Mnayer</t>
+  </si>
+  <si>
+    <t>mal-mnayer@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Kartik Sanjaybhai Sorathiya</t>
+  </si>
+  <si>
+    <t>kssorathiya@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Cleo Buenaventura</t>
+  </si>
+  <si>
+    <t>cjbuenaventura@myseneca.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,13 +1112,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -329,8 +1140,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,8 +1175,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5A6BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -429,11 +1297,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -465,8 +1424,139 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -798,21 +1888,1264 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C5EFC3-9CF6-4304-AECD-C99C36813164}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283E44F7-DBDF-4774-928D-66EF12AA0279}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840DDD99-55A5-45CA-BDD8-12537C8CCEC7}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="93" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="93" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" s="17"/>
+    </row>
+    <row r="20" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46396CA6-995C-41C3-AE24-D161ECDB9B3F}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="36"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF083D4-D14D-4745-B2CE-66771670E000}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B838678E-12C9-4F91-872B-E13857F5E97C}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" ht="106.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" spans="1:8" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="39"/>
+    </row>
+    <row r="5" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="39"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -860,11 +3193,11 @@
         <v>10</v>
       </c>
       <c r="F2" s="5"/>
-      <c r="G2" t="s">
-        <v>59</v>
+      <c r="G2" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
@@ -891,7 +3224,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -908,14 +3241,14 @@
         <v>19</v>
       </c>
       <c r="F4" s="7"/>
-      <c r="G4" t="s">
-        <v>60</v>
+      <c r="G4" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -932,11 +3265,11 @@
         <v>19</v>
       </c>
       <c r="F5" s="7"/>
-      <c r="G5" t="s">
-        <v>61</v>
+      <c r="G5" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -963,7 +3296,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>27</v>
       </c>
@@ -981,10 +3314,10 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
@@ -1005,10 +3338,10 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1029,10 +3362,10 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1053,10 +3386,10 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1077,10 +3410,10 @@
       </c>
       <c r="F11" s="7"/>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1101,13 +3434,13 @@
       </c>
       <c r="F12" s="7"/>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -1125,10 +3458,10 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
@@ -1142,20 +3475,20 @@
         <v>8</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1179,7 +3512,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
@@ -1203,10 +3536,680 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" t="s">
-        <v>57</v>
-      </c>
+    <row r="17" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="43"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{91C0FD8E-F70F-4DDE-B60B-612456B257A8}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{3F84DF2E-48F0-734D-A6A7-380F36779B12}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{297D0F51-9B30-9840-ADA3-5F10E50DCE86}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85BFC73-A50F-4A1D-A3DE-793EB499E494}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>284</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="49"/>
+    </row>
+    <row r="14" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="F14" s="49"/>
+    </row>
+    <row r="15" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>303</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>304</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>280</v>
+      </c>
+      <c r="F15" s="51"/>
+    </row>
+    <row r="16" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>306</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="51" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>310</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D17" s="52" t="s">
+        <v>311</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>312</v>
+      </c>
+      <c r="F17" s="51"/>
+    </row>
+    <row r="18" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>311</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>315</v>
+      </c>
+      <c r="F18" s="51"/>
+    </row>
+    <row r="19" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>311</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="51"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD395CD2-CFDA-46FB-9BE0-FE3BC09B3A5E}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7887C1-1E21-4125-8869-B8ED5CAFAA7A}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="F8" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1215,26 +4218,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="11336436-e19c-451d-b666-d7c312f84b68">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b8d82043-2af1-4b83-b781-b5f1c44103c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFB5B515010BFB41A71EECADA093B687" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579b45423472ebbaf4eed9c56b664d89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="11336436-e19c-451d-b666-d7c312f84b68" xmlns:ns3="b8d82043-2af1-4b83-b781-b5f1c44103c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95cf8f956f3c1dab4d6aa3fe57d77289" ns2:_="" ns3:_="">
     <xsd:import namespace="11336436-e19c-451d-b666-d7c312f84b68"/>
@@ -1447,32 +4430,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE7B145-1F1D-4D31-86E8-4833F892997F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D214C69C-128C-4199-A567-2B301B7A3A01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="11336436-e19c-451d-b666-d7c312f84b68"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b8d82043-2af1-4b83-b781-b5f1c44103c2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="11336436-e19c-451d-b666-d7c312f84b68">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b8d82043-2af1-4b83-b781-b5f1c44103c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2AD03AC-4534-491E-8B93-C2832B09AB86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1489,4 +4467,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE7B145-1F1D-4D31-86E8-4833F892997F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D214C69C-128C-4199-A567-2B301B7A3A01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b8d82043-2af1-4b83-b781-b5f1c44103c2"/>
+    <ds:schemaRef ds:uri="11336436-e19c-451d-b666-d7c312f84b68"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
bug fix, camel casing TS
</commit_message>
<xml_diff>
--- a/excel_input/KEY ORGANIZERS.xlsx
+++ b/excel_input/KEY ORGANIZERS.xlsx
@@ -15,13 +15,14 @@
     <sheet name="MARKETING &amp; COMMUNICATIONS TEAM" sheetId="6" r:id="rId6"/>
     <sheet name="CREATIVES TEAM" sheetId="7" r:id="rId7"/>
     <sheet name="CONSULTANTS" sheetId="8" r:id="rId8"/>
+    <sheet name="ISSUE MANAGEMENT TEAM" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="318">
   <si>
     <t>Name</t>
   </si>
@@ -80,9 +81,6 @@
     <t>Nisal Chandana Ekanayake</t>
   </si>
   <si>
-    <t>Upesha Pankajbhai Patel</t>
-  </si>
-  <si>
     <t>Naitik Pankaj Kumar Raval</t>
   </si>
   <si>
@@ -92,7 +90,7 @@
     <t>Andrea Huesca Enciso</t>
   </si>
   <si>
-    <t>Brenda CÃ¡ceres</t>
+    <t>Brenda Caceres</t>
   </si>
   <si>
     <t>Haru Ai Okabe</t>
@@ -143,9 +141,6 @@
     <t>ncekanayake@myseneca.ca</t>
   </si>
   <si>
-    <t>uppatel8@myseneca.ca</t>
-  </si>
-  <si>
     <t>npkraval@myseneca.ca</t>
   </si>
   <si>
@@ -182,13 +177,13 @@
     <t>Project Manager, Operations</t>
   </si>
   <si>
-    <t>Daily Reports Officer</t>
+    <t>Daily Report Offier</t>
   </si>
   <si>
     <t>Weekly Reports Officer</t>
   </si>
   <si>
-    <t xml:space="preserve">Manager,Â Rules, Regulations, Prizing, and JudgingÂ </t>
+    <t>Manager, Rules, Regulations, Prizing, and Judging</t>
   </si>
   <si>
     <t>Prizing</t>
@@ -209,15 +204,15 @@
     <t xml:space="preserve">Manager, Event Catering </t>
   </si>
   <si>
-    <t>Catering Officer</t>
-  </si>
-  <si>
     <t>Manager, Registrations</t>
   </si>
   <si>
     <t>Registration Officer</t>
   </si>
   <si>
+    <t>Producer</t>
+  </si>
+  <si>
     <t>Broadcast Officer</t>
   </si>
   <si>
@@ -236,9 +231,6 @@
     <t>Business Tech Management</t>
   </si>
   <si>
-    <t>Weekly Operations Updates /Registration Team</t>
-  </si>
-  <si>
     <t>Integration Management / Project Control Officer</t>
   </si>
   <si>
@@ -272,7 +264,7 @@
     <t>Finance</t>
   </si>
   <si>
-    <t xml:space="preserve">Manager,Â Event AccountingÂ </t>
+    <t>Manager, Event Accounting</t>
   </si>
   <si>
     <t>Finance Planning</t>
@@ -515,7 +507,7 @@
     <t xml:space="preserve">  Student Success Director</t>
   </si>
   <si>
-    <t>Challenge Set Liaison / Team Lead â Participant Support</t>
+    <t>Challenge Set Liaison / Team Lead - Participant Support</t>
   </si>
   <si>
     <t>Student Sucess Manager</t>
@@ -587,9 +579,6 @@
     <t>Shanu Anie Alias</t>
   </si>
   <si>
-    <t>Ankit Thapar</t>
-  </si>
-  <si>
     <t>Osman Kahraman</t>
   </si>
   <si>
@@ -635,9 +624,6 @@
     <t>saalias@myseneca.ca</t>
   </si>
   <si>
-    <t>ankit.thapar@senecapolytechnic.ca</t>
-  </si>
-  <si>
     <t>okahraman2@myseneca.ca</t>
   </si>
   <si>
@@ -719,9 +705,6 @@
     <t xml:space="preserve">Shivani Nallamati </t>
   </si>
   <si>
-    <t>Justin Wong</t>
-  </si>
-  <si>
     <t>Talia Ghalayini</t>
   </si>
   <si>
@@ -767,9 +750,6 @@
     <t>nallamatishivani18@gmail.com</t>
   </si>
   <si>
-    <t>jwong301@myseneca.ca</t>
-  </si>
-  <si>
     <t>tghalayini1@myseneca.ca</t>
   </si>
   <si>
@@ -839,9 +819,6 @@
     <t>Business</t>
   </si>
   <si>
-    <t>Public Relations and Communications</t>
-  </si>
-  <si>
     <t>Computer Engineering Technology</t>
   </si>
   <si>
@@ -938,18 +915,6 @@
     <t>Graphics Design</t>
   </si>
   <si>
-    <t>Rishan Mendis</t>
-  </si>
-  <si>
-    <t>Shreya Adhvaryu</t>
-  </si>
-  <si>
-    <t>Shlok Kumar Sharma</t>
-  </si>
-  <si>
-    <t>Arya Prasad Samant</t>
-  </si>
-  <si>
     <t>Majd Al Mnayer</t>
   </si>
   <si>
@@ -959,18 +924,6 @@
     <t>Cleo Buenaventura</t>
   </si>
   <si>
-    <t>rishanmendis@yahoo.com / rmendis1@myseneca.ca</t>
-  </si>
-  <si>
-    <t>shreya.adhvaryu@senecapolytechnic.ca</t>
-  </si>
-  <si>
-    <t>shlok-kumar.sharma@senecapolytechnic.ca</t>
-  </si>
-  <si>
-    <t>aryasamant.10@gmail.com</t>
-  </si>
-  <si>
     <t>mal-mnayer@myseneca.ca</t>
   </si>
   <si>
@@ -980,12 +933,6 @@
     <t>cjbuenaventura@myseneca.ca</t>
   </si>
   <si>
-    <t>Marketing / Partner Experience</t>
-  </si>
-  <si>
-    <t>Social Media Marketing</t>
-  </si>
-  <si>
     <t>IT / Student Success/ First Nations</t>
   </si>
   <si>
@@ -993,6 +940,42 @@
   </si>
   <si>
     <t>BSD</t>
+  </si>
+  <si>
+    <t>Kohulan Thevananthan</t>
+  </si>
+  <si>
+    <t>Isaiah Cyrus Majam</t>
+  </si>
+  <si>
+    <t>Suhana Shrestha</t>
+  </si>
+  <si>
+    <t>kthevananthan@myseneca.ca</t>
+  </si>
+  <si>
+    <t>sshrestha140@myseneca.ca</t>
+  </si>
+  <si>
+    <t>Issues Management</t>
+  </si>
+  <si>
+    <t>Issue Management Director</t>
+  </si>
+  <si>
+    <t>Partner Experience Director</t>
+  </si>
+  <si>
+    <t>Events Director</t>
+  </si>
+  <si>
+    <t>Chief of Staff</t>
+  </si>
+  <si>
+    <t>PMCC</t>
+  </si>
+  <si>
+    <t>To be filled</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1333,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1387,16 +1370,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1404,16 +1387,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1421,19 +1404,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1441,19 +1421,19 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1461,19 +1441,19 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1481,19 +1461,19 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1501,19 +1481,19 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1521,16 +1501,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1538,19 +1518,19 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1558,19 +1538,19 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1578,16 +1558,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1595,16 +1575,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>74</v>
@@ -1615,19 +1595,19 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1635,19 +1615,19 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1655,19 +1635,19 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1675,19 +1655,19 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1695,19 +1675,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1715,7 +1683,7 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1723,7 +1691,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1731,36 +1708,19 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
       <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" t="s">
-        <v>79</v>
+      <c r="F21" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1804,19 +1764,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1860,201 +1820,201 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
         <v>105</v>
       </c>
-      <c r="C11" t="s">
-        <v>108</v>
-      </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2098,311 +2058,311 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" t="s">
         <v>162</v>
       </c>
-      <c r="D4" t="s">
-        <v>165</v>
-      </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E14" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
         <v>159</v>
       </c>
-      <c r="C17" t="s">
-        <v>162</v>
-      </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2412,7 +2372,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2446,274 +2406,257 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" t="s">
         <v>212</v>
       </c>
-      <c r="D6" t="s">
-        <v>217</v>
-      </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" t="s">
         <v>206</v>
       </c>
-      <c r="C13" t="s">
-        <v>211</v>
-      </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" t="s">
         <v>211</v>
       </c>
-      <c r="D14" t="s">
-        <v>217</v>
-      </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" t="s">
         <v>211</v>
       </c>
-      <c r="D15" t="s">
-        <v>216</v>
-      </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" t="s">
-        <v>210</v>
-      </c>
-      <c r="C17" t="s">
-        <v>211</v>
-      </c>
-      <c r="D17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2723,7 +2666,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2757,295 +2700,278 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" t="s">
         <v>269</v>
-      </c>
-      <c r="F2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F3" t="s">
         <v>270</v>
-      </c>
-      <c r="F3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F4" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E5" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C6" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D7" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C8" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E8" t="s">
-        <v>272</v>
+        <v>265</v>
+      </c>
+      <c r="F8" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E9" t="s">
-        <v>273</v>
-      </c>
-      <c r="F9" t="s">
-        <v>279</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" t="s">
         <v>258</v>
       </c>
-      <c r="D10" t="s">
-        <v>264</v>
-      </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="F10" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" t="s">
         <v>251</v>
       </c>
-      <c r="C11" t="s">
-        <v>258</v>
-      </c>
       <c r="D11" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E12" t="s">
-        <v>269</v>
+        <v>115</v>
+      </c>
+      <c r="F12" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B13" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C13" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C14" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E14" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C15" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E15" t="s">
-        <v>275</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B16" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C16" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D16" t="s">
+        <v>261</v>
+      </c>
+      <c r="E16" t="s">
         <v>268</v>
-      </c>
-      <c r="E16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>241</v>
-      </c>
-      <c r="B17" t="s">
-        <v>257</v>
-      </c>
-      <c r="C17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D17" t="s">
-        <v>268</v>
-      </c>
-      <c r="E17" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3089,121 +3015,121 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" t="s">
         <v>289</v>
       </c>
-      <c r="C2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D2" t="s">
-        <v>297</v>
-      </c>
       <c r="E2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D3" t="s">
         <v>290</v>
       </c>
-      <c r="C3" t="s">
-        <v>296</v>
-      </c>
-      <c r="D3" t="s">
-        <v>298</v>
-      </c>
       <c r="E3" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" t="s">
         <v>291</v>
       </c>
-      <c r="C4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D4" t="s">
-        <v>299</v>
-      </c>
       <c r="E4" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D5" t="s">
         <v>292</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>296</v>
-      </c>
-      <c r="D5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E5" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" t="s">
         <v>293</v>
       </c>
-      <c r="C6" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" t="s">
-        <v>301</v>
-      </c>
       <c r="E6" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" t="s">
         <v>294</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>296</v>
-      </c>
-      <c r="D7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E7" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" t="s">
         <v>288</v>
       </c>
-      <c r="B8" t="s">
-        <v>295</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E8" t="s">
         <v>296</v>
-      </c>
-      <c r="D8" t="s">
-        <v>302</v>
-      </c>
-      <c r="E8" t="s">
-        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3213,7 +3139,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3247,36 +3173,129 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" t="s">
         <v>305</v>
-      </c>
-      <c r="B2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>306</v>
       </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
       <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D3" t="s">
         <v>313</v>
       </c>
-      <c r="C3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" t="s">
-        <v>322</v>
-      </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>113</v>
+      </c>
+      <c r="F3" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3284,16 +3303,19 @@
         <v>307</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" t="s">
         <v>314</v>
       </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>322</v>
-      </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3301,67 +3323,19 @@
         <v>308</v>
       </c>
       <c r="B5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D5" t="s">
         <v>315</v>
       </c>
-      <c r="C5" t="s">
-        <v>320</v>
-      </c>
-      <c r="D5" t="s">
-        <v>322</v>
-      </c>
       <c r="E5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>309</v>
-      </c>
-      <c r="B6" t="s">
         <v>316</v>
       </c>
-      <c r="C6" t="s">
-        <v>321</v>
-      </c>
-      <c r="D6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>310</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="F5" t="s">
         <v>317</v>
-      </c>
-      <c r="C7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" t="s">
-        <v>322</v>
-      </c>
-      <c r="E7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>311</v>
-      </c>
-      <c r="B8" t="s">
-        <v>318</v>
-      </c>
-      <c r="C8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" t="s">
-        <v>322</v>
-      </c>
-      <c r="E8" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>